<commit_message>
Planning voor komende weken ingevuld. Taken moeten nog verdeeld worden. naamgeving constraints model verbeterd.
</commit_message>
<xml_diff>
--- a/Map tijdelijke documenten/Plan van aanpak/MoSCoW Planning.xlsx
+++ b/Map tijdelijke documenten/Plan van aanpak/MoSCoW Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="20730" windowHeight="11700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_GoBack" localSheetId="0">Sheet1!$A$26</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -93,12 +93,6 @@
     <t>webinterface/UI</t>
   </si>
   <si>
-    <t xml:space="preserve">      2e scherm met verdere informatie over gekozen was programma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Instelbare knopen voor de tempratuur. </t>
-  </si>
-  <si>
     <t>en mogelijke anderen instellingen voor was programma</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t xml:space="preserve">     Updaten van web interface/WM. </t>
   </si>
   <si>
-    <t xml:space="preserve">      Grote knopen voor selectie van was programma.</t>
-  </si>
-  <si>
     <t>scherm word geopend na selectie was programma</t>
   </si>
   <si>
@@ -157,15 +148,31 @@
   </si>
   <si>
     <t xml:space="preserve">     Het uitvoeren van verschillende was programma's.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Instelbare knoppen voor de temperatuur. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      2e scherm met verdere informatie over gekozen wasprogramma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Grote knoppen voor selectie van wasprogramma.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -344,129 +351,130 @@
   </borders>
   <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="15" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="63">
@@ -869,7 +877,7 @@
   <dimension ref="A1:Q1048573"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1090,7 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="32"/>
@@ -1094,11 +1102,11 @@
       <c r="Q14" s="20"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>36</v>
+      <c r="A15" s="38" t="s">
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="33"/>
       <c r="D15" s="32"/>
@@ -1112,10 +1120,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="33"/>
@@ -1128,11 +1136,11 @@
       <c r="Q16" s="20"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
-        <v>23</v>
+      <c r="A17" s="38" t="s">
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="32"/>
@@ -1145,11 +1153,11 @@
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>24</v>
+      <c r="A18" s="38" t="s">
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="33"/>
@@ -1163,7 +1171,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="32"/>
@@ -1178,7 +1186,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="33"/>
@@ -1190,7 +1198,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="33"/>
@@ -1201,10 +1209,10 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C22" s="32"/>
       <c r="D22" s="33"/>
@@ -1215,10 +1223,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C23" s="32"/>
       <c r="D23" s="32"/>
@@ -1229,7 +1237,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="32"/>
@@ -1241,7 +1249,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
@@ -1252,7 +1260,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="36"/>
@@ -1263,7 +1271,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C27" s="36"/>
       <c r="D27" s="33"/>
@@ -1275,7 +1283,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="36"/>
@@ -1296,7 +1304,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="32"/>

</xml_diff>